<commit_message>
Corrected search component to fit home page
</commit_message>
<xml_diff>
--- a/uploads/0783975669_MoMo_Transaction.xlsx
+++ b/uploads/0783975669_MoMo_Transaction.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHEMA Valentin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHEMA Valentin\Desktop\Momo_statement\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1295,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1310,7 +1310,7 @@
     <col min="7" max="7" width="23.59765625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.69921875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="7.69921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.296875" customWidth="1"/>
+    <col min="11" max="11" width="8.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3">
-        <v>3900</v>
+        <v>-3900</v>
       </c>
       <c r="J5" s="3">
         <v>10</v>
@@ -1570,7 +1570,7 @@
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3">
-        <v>2500</v>
+        <v>-2500</v>
       </c>
       <c r="J8" s="3">
         <v>10</v>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3">
-        <v>600</v>
+        <v>-600</v>
       </c>
       <c r="J10" s="3">
         <v>10</v>
@@ -1702,7 +1702,7 @@
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="J12" s="3">
         <v>10</v>
@@ -1834,7 +1834,7 @@
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3">
-        <v>800</v>
+        <v>-800</v>
       </c>
       <c r="J16" s="3">
         <v>710</v>
@@ -1867,7 +1867,7 @@
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3">
-        <v>300</v>
+        <v>-300</v>
       </c>
       <c r="J17" s="3">
         <v>410</v>
@@ -1902,7 +1902,7 @@
         <v>20</v>
       </c>
       <c r="I18" s="3">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="J18" s="3">
         <v>240</v>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3">
-        <v>200</v>
+        <v>-200</v>
       </c>
       <c r="J19" s="3">
         <v>40</v>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="J21" s="3">
         <v>40</v>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3">
-        <v>400</v>
+        <v>-400</v>
       </c>
       <c r="J23" s="3">
         <v>140</v>
@@ -2100,7 +2100,7 @@
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="J24" s="3">
         <v>40</v>
@@ -2168,7 +2168,7 @@
         <v>20</v>
       </c>
       <c r="I26" s="3">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="J26" s="3">
         <v>70</v>
@@ -2762,7 +2762,7 @@
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3">
-        <v>500000</v>
+        <v>-500000</v>
       </c>
       <c r="J44" s="3">
         <v>22080</v>
@@ -2830,7 +2830,7 @@
         <v>20</v>
       </c>
       <c r="I46" s="3">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="J46" s="3">
         <v>72010</v>
@@ -2865,7 +2865,7 @@
         <v>20</v>
       </c>
       <c r="I47" s="3">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="J47" s="3">
         <v>71890</v>
@@ -3032,7 +3032,7 @@
         <v>20</v>
       </c>
       <c r="I52" s="3">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="J52" s="3">
         <v>104710</v>
@@ -3430,7 +3430,7 @@
         <v>2000</v>
       </c>
       <c r="I64" s="3">
-        <v>115000</v>
+        <v>-115000</v>
       </c>
       <c r="J64" s="3">
         <v>28830</v>
@@ -3465,7 +3465,7 @@
         <v>120</v>
       </c>
       <c r="I65" s="3">
-        <v>2500</v>
+        <v>-2500</v>
       </c>
       <c r="J65" s="3">
         <v>26210</v>
@@ -3498,7 +3498,7 @@
       </c>
       <c r="H66" s="3"/>
       <c r="I66" s="3">
-        <v>21500</v>
+        <v>-21500</v>
       </c>
       <c r="J66" s="3">
         <v>4710</v>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="H67" s="3"/>
       <c r="I67" s="3">
-        <v>4500</v>
+        <v>-4500</v>
       </c>
       <c r="J67" s="3">
         <v>210</v>

</xml_diff>